<commit_message>
Actualización de Instituciones Colaboradoras
</commit_message>
<xml_diff>
--- a/SCIA_INSTITUCIONES.xlsx
+++ b/SCIA_INSTITUCIONES.xlsx
@@ -1,28 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbugueno\Desktop\BBDD_DEGE\Colaboracion_Institucional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://portalconicyt-my.sharepoint.com/personal/carenas_anid_cl/Documents/Escritorio/Github ANID/Colaboracion_Institucional/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_717211C6E78BA29A9BC5CF60FE9BEDEB3DF826EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98CF1D26-563D-4236-BFF9-A56B52CC2874}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCIA_INSTITUCIONES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SCIA_INSTITUCIONES!$A$1:$L$925</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SCIA_INSTITUCIONES!$A$1:$L$1237</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12367" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12677" uniqueCount="1089">
   <si>
     <t>PROGRAMA</t>
   </si>
@@ -3205,12 +3219,96 @@
   </si>
   <si>
     <t>MAROUN KHOURY</t>
+  </si>
+  <si>
+    <t>CONCURSO APOYO CENTROS DE EXCELENCIA CON FINANCIAMIENTO BASAL 2022</t>
+  </si>
+  <si>
+    <t>AFB220001</t>
+  </si>
+  <si>
+    <t>AFB220002</t>
+  </si>
+  <si>
+    <t>AFB220003</t>
+  </si>
+  <si>
+    <t>AFB220004</t>
+  </si>
+  <si>
+    <t>1522A0001</t>
+  </si>
+  <si>
+    <t>RENE GARREAUD SALAZAR</t>
+  </si>
+  <si>
+    <t>1522A0002</t>
+  </si>
+  <si>
+    <t>WALDO BUSTAMANTE GOMEZ</t>
+  </si>
+  <si>
+    <t>1522A0003</t>
+  </si>
+  <si>
+    <t>PEDRO MEGE ROSSO</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD ACADEMIA DE HUMANISMO CRISTIANO</t>
+  </si>
+  <si>
+    <t>71470400-1</t>
+  </si>
+  <si>
+    <t>1522A0004</t>
+  </si>
+  <si>
+    <t>RENATO QUIÑONES BERGERET</t>
+  </si>
+  <si>
+    <t>1522A0005</t>
+  </si>
+  <si>
+    <t>RODRIGO CIENFUEGOS CARRASCO</t>
+  </si>
+  <si>
+    <t>1522A0006</t>
+  </si>
+  <si>
+    <t>CLAUDIA RAHMANN ZUÑIGA</t>
+  </si>
+  <si>
+    <t>CONCURSO DE APOYO A CENTROS DE EXCELENCIA EN INVESTIGACION EN AREAS PRIORITARIAS - FONDAP 2022</t>
+  </si>
+  <si>
+    <t>APOYO AL FORTALECIMIENTO A LAS CAPACIDADES PARA I+D 2022 MODALIDAD CENTROS TECNOLOGICOS PARA LA INNOVACION Y CENTROS DE EXCELENCIA INTERNACIONAL</t>
+  </si>
+  <si>
+    <t>CTI220001</t>
+  </si>
+  <si>
+    <t>MAY CHOMALI GARIB</t>
+  </si>
+  <si>
+    <t>CENTRO</t>
+  </si>
+  <si>
+    <t>CENTRO NACIONAL DE SISTEMAS DE                    INFORMACION EN SALUD</t>
+  </si>
+  <si>
+    <t>65165006-2</t>
+  </si>
+  <si>
+    <t>CTI220002</t>
+  </si>
+  <si>
+    <t>NAYAT SANCHEZ PI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4010,12 +4108,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1237"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1186" sqref="F1186"/>
+      <pane ySplit="1" topLeftCell="A1245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1269" sqref="A1269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51026,6 +51124,1184 @@
         <v>853</v>
       </c>
     </row>
+    <row r="1238" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1238" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D1238">
+        <v>2022</v>
+      </c>
+      <c r="E1238">
+        <v>2022</v>
+      </c>
+      <c r="F1238" t="s">
+        <v>744</v>
+      </c>
+      <c r="G1238" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1238" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1238" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1238" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1238" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1238" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1239" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D1239">
+        <v>2022</v>
+      </c>
+      <c r="E1239">
+        <v>2022</v>
+      </c>
+      <c r="F1239" t="s">
+        <v>744</v>
+      </c>
+      <c r="G1239" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1239" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I1239" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1239" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1239" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1239" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1240" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D1240">
+        <v>2022</v>
+      </c>
+      <c r="E1240">
+        <v>2022</v>
+      </c>
+      <c r="F1240" t="s">
+        <v>744</v>
+      </c>
+      <c r="G1240" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1240" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1240" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1240" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1240" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1240" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1241" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D1241">
+        <v>2022</v>
+      </c>
+      <c r="E1241">
+        <v>2022</v>
+      </c>
+      <c r="F1241" t="s">
+        <v>643</v>
+      </c>
+      <c r="G1241" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1241" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I1241" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1241" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1241" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1241" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1242" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1242" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D1242">
+        <v>2022</v>
+      </c>
+      <c r="E1242">
+        <v>2022</v>
+      </c>
+      <c r="F1242" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1242" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1242" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I1242" t="s">
+        <v>414</v>
+      </c>
+      <c r="J1242" t="s">
+        <v>415</v>
+      </c>
+      <c r="K1242" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1242" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1243" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1243" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D1243">
+        <v>2022</v>
+      </c>
+      <c r="E1243">
+        <v>2022</v>
+      </c>
+      <c r="F1243" t="s">
+        <v>747</v>
+      </c>
+      <c r="G1243" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1243" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I1243" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1243" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1243" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1243" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1244" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1244" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D1244">
+        <v>2022</v>
+      </c>
+      <c r="E1244">
+        <v>2022</v>
+      </c>
+      <c r="F1244" t="s">
+        <v>1067</v>
+      </c>
+      <c r="G1244" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1244" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1244" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1244" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1244" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1244" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1245" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D1245">
+        <v>2022</v>
+      </c>
+      <c r="E1245">
+        <v>2022</v>
+      </c>
+      <c r="F1245" t="s">
+        <v>1067</v>
+      </c>
+      <c r="G1245" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1245" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1245" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1245" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1245" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1245" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1246" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1246" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D1246">
+        <v>2022</v>
+      </c>
+      <c r="E1246">
+        <v>2022</v>
+      </c>
+      <c r="F1246" t="s">
+        <v>1067</v>
+      </c>
+      <c r="G1246" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1246" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1246" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1246" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1246" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1246" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1247" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1247" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D1247">
+        <v>2022</v>
+      </c>
+      <c r="E1247">
+        <v>2022</v>
+      </c>
+      <c r="F1247" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G1247" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1247" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1247" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1247" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1247" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1247" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1248" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1248" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D1248">
+        <v>2022</v>
+      </c>
+      <c r="E1248">
+        <v>2022</v>
+      </c>
+      <c r="F1248" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G1248" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1248" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1248" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1248" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1248" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1248" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1249" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1249" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D1249">
+        <v>2022</v>
+      </c>
+      <c r="E1249">
+        <v>2022</v>
+      </c>
+      <c r="F1249" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G1249" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1249" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1249" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1249" t="s">
+        <v>275</v>
+      </c>
+      <c r="K1249" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1249" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1250" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1250" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D1250">
+        <v>2022</v>
+      </c>
+      <c r="E1250">
+        <v>2022</v>
+      </c>
+      <c r="F1250" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G1250" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1250" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1250" t="s">
+        <v>1072</v>
+      </c>
+      <c r="J1250" t="s">
+        <v>1073</v>
+      </c>
+      <c r="K1250" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1250" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1251" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1251" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D1251">
+        <v>2022</v>
+      </c>
+      <c r="E1251">
+        <v>2022</v>
+      </c>
+      <c r="F1251" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G1251" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1251" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1251" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1251" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1251" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1251" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1252" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1252" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D1252">
+        <v>2022</v>
+      </c>
+      <c r="E1252">
+        <v>2022</v>
+      </c>
+      <c r="F1252" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G1252" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1252" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1252" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1252" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1252" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1252" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1253" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1253" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D1253">
+        <v>2022</v>
+      </c>
+      <c r="E1253">
+        <v>2022</v>
+      </c>
+      <c r="F1253" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G1253" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1253" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1253" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1253" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1253" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1253" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1254" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1254" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D1254">
+        <v>2022</v>
+      </c>
+      <c r="E1254">
+        <v>2022</v>
+      </c>
+      <c r="F1254" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G1254" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1254" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1254" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1254" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1254" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1254" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1255" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1255" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D1255">
+        <v>2022</v>
+      </c>
+      <c r="E1255">
+        <v>2022</v>
+      </c>
+      <c r="F1255" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1255" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1255" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1255" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1255" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1255" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1255" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1256" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1256" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D1256">
+        <v>2022</v>
+      </c>
+      <c r="E1256">
+        <v>2022</v>
+      </c>
+      <c r="F1256" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1256" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1256" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1256" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1256" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1256" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1256" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1257" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1257" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D1257">
+        <v>2022</v>
+      </c>
+      <c r="E1257">
+        <v>2022</v>
+      </c>
+      <c r="F1257" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1257" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1257" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1257" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1257" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1257" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1257" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1258" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1258" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D1258">
+        <v>2022</v>
+      </c>
+      <c r="E1258">
+        <v>2022</v>
+      </c>
+      <c r="F1258" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1258" t="s">
+        <v>781</v>
+      </c>
+      <c r="H1258" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1258" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1258" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1258" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1258" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1259" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1259" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1259">
+        <v>2022</v>
+      </c>
+      <c r="E1259">
+        <v>2022</v>
+      </c>
+      <c r="F1259" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1259" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1259" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1259" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1259" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1259" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1259" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1260" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1260" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1260">
+        <v>2022</v>
+      </c>
+      <c r="E1260">
+        <v>2022</v>
+      </c>
+      <c r="F1260" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1260" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1260" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1260" t="s">
+        <v>179</v>
+      </c>
+      <c r="J1260" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1260" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1260" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1261" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1261" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1261">
+        <v>2022</v>
+      </c>
+      <c r="E1261">
+        <v>2022</v>
+      </c>
+      <c r="F1261" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1261" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1261" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1261" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1261" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1261" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1261" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1262" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1262" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1262">
+        <v>2022</v>
+      </c>
+      <c r="E1262">
+        <v>2022</v>
+      </c>
+      <c r="F1262" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1262" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1262" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1262" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1262" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1262" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1262" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1263" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1263" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1263">
+        <v>2022</v>
+      </c>
+      <c r="E1263">
+        <v>2022</v>
+      </c>
+      <c r="F1263" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1263" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1263" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1263" t="s">
+        <v>444</v>
+      </c>
+      <c r="J1263" t="s">
+        <v>238</v>
+      </c>
+      <c r="K1263" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1263" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1264" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1264" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1264">
+        <v>2022</v>
+      </c>
+      <c r="E1264">
+        <v>2022</v>
+      </c>
+      <c r="F1264" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1264" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1264" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1264" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1264" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1264" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1264" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1265" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1265" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1265">
+        <v>2022</v>
+      </c>
+      <c r="E1265">
+        <v>2022</v>
+      </c>
+      <c r="F1265" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1265" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1265" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1265" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1265" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1265" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1265" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1266" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1266" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1266">
+        <v>2022</v>
+      </c>
+      <c r="E1266">
+        <v>2022</v>
+      </c>
+      <c r="F1266" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G1266" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1266" t="s">
+        <v>784</v>
+      </c>
+      <c r="I1266" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1266" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1266" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1266" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1267" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1267" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D1267">
+        <v>2022</v>
+      </c>
+      <c r="E1267">
+        <v>2022</v>
+      </c>
+      <c r="F1267" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G1267" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1267" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I1267" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J1267" t="s">
+        <v>1086</v>
+      </c>
+      <c r="K1267" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1267" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1268" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1268" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D1268">
+        <v>2022</v>
+      </c>
+      <c r="E1268">
+        <v>2022</v>
+      </c>
+      <c r="F1268" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G1268" t="s">
+        <v>780</v>
+      </c>
+      <c r="H1268" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I1268" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J1268" t="s">
+        <v>1029</v>
+      </c>
+      <c r="K1268" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1268" t="s">
+        <v>857</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>